<commit_message>
Updates for 4 April
</commit_message>
<xml_diff>
--- a/20-04_03 world o meter adjusted covid cases by state.xlsx
+++ b/20-04_03 world o meter adjusted covid cases by state.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/71ffaa969b2b2dbb/Meridian/h Computer Science/Teacher Projects/COVID/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{C78C712A-4E04-47A1-8C52-548FE065773B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5934B35F-9A8D-4976-9024-AD2A242B5D54}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="8_{C78C712A-4E04-47A1-8C52-548FE065773B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3EBD055B-42C9-40E1-98F8-DF76FD2A28C1}"/>
   <bookViews>
-    <workbookView xWindow="8835" yWindow="-19185" windowWidth="27615" windowHeight="16290" activeTab="1" xr2:uid="{C2EC3F12-84D7-4DDA-AADC-120E6E7C982F}"/>
+    <workbookView xWindow="17940" yWindow="-18075" windowWidth="15030" windowHeight="16290" xr2:uid="{C2EC3F12-84D7-4DDA-AADC-120E6E7C982F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -438,7 +438,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
@@ -488,6 +488,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -496,12 +499,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -822,8 +819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FB61549-E677-4976-9DCA-747A592A5594}">
   <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:D59"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5:G59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -833,27 +830,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="H1" s="21"/>
+      <c r="H1" s="22"/>
       <c r="I1" s="8">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="21.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="20"/>
-      <c r="H2" s="19" t="s">
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="21"/>
+      <c r="H2" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="I2" s="19"/>
+      <c r="I2" s="20"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
@@ -914,24 +911,24 @@
         <v>7</v>
       </c>
       <c r="B5" s="1">
-        <v>93053</v>
+        <v>103476</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="1">
-        <v>2538</v>
+        <v>3218</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="1">
-        <v>83081</v>
+        <v>91372</v>
       </c>
       <c r="G5" s="9"/>
       <c r="H5" s="6">
         <f>D5/$I$1</f>
-        <v>195230.76923076925</v>
+        <v>247538.46153846156</v>
       </c>
       <c r="I5" s="7">
         <f>ABS(F5-H5)/H5</f>
-        <v>0.5744472025216707</v>
+        <v>0.63087756370416415</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -939,153 +936,153 @@
         <v>8</v>
       </c>
       <c r="B6" s="1">
-        <v>25590</v>
+        <v>29895</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2">
-        <v>537</v>
+        <v>646</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="1">
-        <v>25053</v>
+        <v>29249</v>
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="6">
         <f t="shared" ref="H6:H53" si="0">D6/$I$1</f>
-        <v>41307.692307692312</v>
+        <v>49692.307692307695</v>
       </c>
       <c r="I6" s="7">
         <f t="shared" ref="I6:I53" si="1">ABS(F6-H6)/H6</f>
-        <v>0.39350279329608945</v>
+        <v>0.41139783281733749</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B7" s="1">
-        <v>11207</v>
-      </c>
-      <c r="C7" s="4">
-        <v>369</v>
-      </c>
+        <v>12744</v>
+      </c>
+      <c r="C7" s="2"/>
       <c r="D7" s="2">
-        <v>246</v>
-      </c>
-      <c r="E7" s="3">
-        <v>12</v>
-      </c>
+        <v>479</v>
+      </c>
+      <c r="E7" s="2"/>
       <c r="F7" s="1">
-        <v>10111</v>
-      </c>
-      <c r="G7" s="10"/>
+        <v>12260</v>
+      </c>
+      <c r="G7" s="9"/>
       <c r="H7" s="6">
         <f t="shared" si="0"/>
-        <v>18923.076923076926</v>
+        <v>36846.153846153851</v>
       </c>
       <c r="I7" s="7">
         <f t="shared" si="1"/>
-        <v>0.46567886178861795</v>
+        <v>0.66726513569937373</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" s="1">
-        <v>10791</v>
-      </c>
-      <c r="C8" s="2"/>
+        <v>12581</v>
+      </c>
+      <c r="C8" s="4">
+        <v>314</v>
+      </c>
       <c r="D8" s="2">
-        <v>417</v>
-      </c>
-      <c r="E8" s="2"/>
+        <v>285</v>
+      </c>
+      <c r="E8" s="3">
+        <v>10</v>
+      </c>
       <c r="F8" s="1">
-        <v>10369</v>
+        <v>11446</v>
       </c>
       <c r="G8" s="9"/>
       <c r="H8" s="6">
         <f t="shared" si="0"/>
-        <v>32076.923076923078</v>
+        <v>21923.076923076926</v>
       </c>
       <c r="I8" s="7">
         <f t="shared" si="1"/>
-        <v>0.67674580335731416</v>
+        <v>0.47790175438596499</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B9" s="1">
-        <v>9150</v>
+        <v>10402</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2">
-        <v>310</v>
+        <v>192</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="1">
-        <v>8820</v>
-      </c>
-      <c r="G9" s="10"/>
+        <v>10200</v>
+      </c>
+      <c r="G9" s="9"/>
       <c r="H9" s="6">
         <f t="shared" si="0"/>
-        <v>23846.153846153848</v>
+        <v>14769.23076923077</v>
       </c>
       <c r="I9" s="7">
         <f t="shared" si="1"/>
-        <v>0.63012903225806449</v>
+        <v>0.30937500000000001</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B10" s="1">
-        <v>9008</v>
+        <v>10297</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2">
-        <v>144</v>
+        <v>370</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="1">
-        <v>8864</v>
-      </c>
-      <c r="G10" s="9"/>
+        <v>9907</v>
+      </c>
+      <c r="G10" s="10"/>
       <c r="H10" s="6">
         <f t="shared" si="0"/>
-        <v>11076.923076923078</v>
+        <v>28461.538461538465</v>
       </c>
       <c r="I10" s="7">
         <f t="shared" si="1"/>
-        <v>0.19977777777777786</v>
+        <v>0.6519162162162162</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B11" s="1">
-        <v>8966</v>
+        <v>10268</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2">
-        <v>154</v>
+        <v>170</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="1">
-        <v>8802</v>
+        <v>10098</v>
       </c>
       <c r="G11" s="9"/>
       <c r="H11" s="6">
         <f t="shared" si="0"/>
-        <v>11846.153846153848</v>
+        <v>13076.923076923078</v>
       </c>
       <c r="I11" s="7">
         <f t="shared" si="1"/>
-        <v>0.25697402597402608</v>
+        <v>0.22780000000000006</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1093,24 +1090,24 @@
         <v>12</v>
       </c>
       <c r="B12" s="1">
-        <v>7695</v>
+        <v>8904</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2">
-        <v>157</v>
+        <v>210</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="1">
-        <v>7536</v>
+        <v>8692</v>
       </c>
       <c r="G12" s="9"/>
       <c r="H12" s="6">
         <f t="shared" si="0"/>
-        <v>12076.923076923078</v>
+        <v>16153.846153846154</v>
       </c>
       <c r="I12" s="7">
         <f t="shared" si="1"/>
-        <v>0.37600000000000006</v>
+        <v>0.46192380952380951</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1118,24 +1115,24 @@
         <v>19</v>
       </c>
       <c r="B13" s="1">
-        <v>7264</v>
+        <v>8420</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="1">
-        <v>7136</v>
+        <v>8280</v>
       </c>
       <c r="G13" s="9"/>
       <c r="H13" s="6">
         <f t="shared" si="0"/>
-        <v>6923.0769230769238</v>
+        <v>7846.1538461538466</v>
       </c>
       <c r="I13" s="7">
         <f t="shared" si="1"/>
-        <v>3.0755555555555453E-2</v>
+        <v>5.5294117647058758E-2</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1143,24 +1140,24 @@
         <v>9</v>
       </c>
       <c r="B14" s="1">
-        <v>6585</v>
+        <v>6966</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2">
-        <v>272</v>
+        <v>291</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="1">
-        <v>5750</v>
+        <v>6112</v>
       </c>
       <c r="G14" s="9"/>
       <c r="H14" s="6">
         <f t="shared" si="0"/>
-        <v>20923.076923076926</v>
+        <v>22384.615384615387</v>
       </c>
       <c r="I14" s="7">
         <f t="shared" si="1"/>
-        <v>0.7251838235294118</v>
+        <v>0.72695532646048111</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1168,28 +1165,24 @@
         <v>16</v>
       </c>
       <c r="B15" s="1">
-        <v>5444</v>
-      </c>
-      <c r="C15" s="4">
-        <v>96</v>
-      </c>
+        <v>5967</v>
+      </c>
+      <c r="C15" s="2"/>
       <c r="D15" s="2">
-        <v>176</v>
-      </c>
-      <c r="E15" s="3">
-        <v>13</v>
-      </c>
+        <v>198</v>
+      </c>
+      <c r="E15" s="2"/>
       <c r="F15" s="1">
-        <v>5268</v>
+        <v>5769</v>
       </c>
       <c r="G15" s="9"/>
       <c r="H15" s="6">
         <f t="shared" si="0"/>
-        <v>13538.461538461539</v>
+        <v>15230.769230769232</v>
       </c>
       <c r="I15" s="7">
         <f t="shared" si="1"/>
-        <v>0.61088636363636362</v>
+        <v>0.62122727272727274</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1197,24 +1190,24 @@
         <v>15</v>
       </c>
       <c r="B16" s="1">
-        <v>4823</v>
+        <v>5658</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2">
-        <v>77</v>
+        <v>97</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="1">
-        <v>4639</v>
+        <v>5311</v>
       </c>
       <c r="G16" s="9"/>
       <c r="H16" s="6">
         <f t="shared" si="0"/>
-        <v>5923.0769230769238</v>
+        <v>7461.5384615384619</v>
       </c>
       <c r="I16" s="7">
         <f t="shared" si="1"/>
-        <v>0.2167922077922079</v>
+        <v>0.28821649484536088</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1222,24 +1215,24 @@
         <v>23</v>
       </c>
       <c r="B17" s="1">
-        <v>3824</v>
+        <v>4914</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2">
-        <v>112</v>
+        <v>131</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="1">
-        <v>3712</v>
+        <v>4783</v>
       </c>
       <c r="G17" s="9"/>
       <c r="H17" s="6">
         <f t="shared" si="0"/>
-        <v>8615.3846153846152</v>
+        <v>10076.923076923078</v>
       </c>
       <c r="I17" s="7">
         <f t="shared" si="1"/>
-        <v>0.56914285714285717</v>
+        <v>0.52535114503816804</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1247,99 +1240,99 @@
         <v>18</v>
       </c>
       <c r="B18" s="1">
-        <v>3728</v>
+        <v>4173</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2">
-        <v>97</v>
+        <v>111</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="1">
-        <v>3631</v>
+        <v>4062</v>
       </c>
       <c r="G18" s="10"/>
       <c r="H18" s="6">
         <f t="shared" si="0"/>
-        <v>7461.5384615384619</v>
+        <v>8538.461538461539</v>
       </c>
       <c r="I18" s="7">
         <f t="shared" si="1"/>
-        <v>0.51337113402061862</v>
+        <v>0.52427027027027029</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="5" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B19" s="1">
-        <v>3194</v>
+        <v>3437</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2">
-        <v>32</v>
+        <v>102</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="1">
-        <v>2942</v>
+        <v>3335</v>
       </c>
       <c r="G19" s="9"/>
       <c r="H19" s="6">
         <f t="shared" si="0"/>
-        <v>2461.5384615384614</v>
+        <v>7846.1538461538466</v>
       </c>
       <c r="I19" s="7">
         <f t="shared" si="1"/>
-        <v>0.19518750000000004</v>
+        <v>0.57495098039215686</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="5" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B20" s="1">
-        <v>3039</v>
+        <v>3312</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="1">
-        <v>2961</v>
+        <v>3221</v>
       </c>
       <c r="G20" s="10"/>
       <c r="H20" s="6">
         <f t="shared" si="0"/>
-        <v>6000</v>
+        <v>7000</v>
       </c>
       <c r="I20" s="7">
         <f t="shared" si="1"/>
-        <v>0.50649999999999995</v>
+        <v>0.53985714285714281</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" s="1">
-        <v>2902</v>
+        <v>3194</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2">
-        <v>81</v>
+        <v>37</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="1">
-        <v>2821</v>
-      </c>
-      <c r="G21" s="10"/>
+        <v>2909</v>
+      </c>
+      <c r="G21" s="9"/>
       <c r="H21" s="6">
         <f t="shared" si="0"/>
-        <v>6230.7692307692314</v>
+        <v>2846.1538461538462</v>
       </c>
       <c r="I21" s="7">
         <f t="shared" si="1"/>
-        <v>0.54724691358024691</v>
+        <v>2.2081081081081068E-2</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1347,24 +1340,24 @@
         <v>26</v>
       </c>
       <c r="B22" s="1">
-        <v>2331</v>
+        <v>2758</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="1">
-        <v>2214</v>
+        <v>2557</v>
       </c>
       <c r="G22" s="10"/>
       <c r="H22" s="6">
         <f t="shared" si="0"/>
-        <v>2769.2307692307695</v>
+        <v>3230.7692307692309</v>
       </c>
       <c r="I22" s="7">
         <f t="shared" si="1"/>
-        <v>0.20050000000000007</v>
+        <v>0.20854761904761909</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1372,24 +1365,28 @@
         <v>24</v>
       </c>
       <c r="B23" s="1">
-        <v>2023</v>
-      </c>
-      <c r="C23" s="2"/>
+        <v>2328</v>
+      </c>
+      <c r="C23" s="4">
+        <v>41</v>
+      </c>
       <c r="D23" s="2">
-        <v>18</v>
-      </c>
-      <c r="E23" s="2"/>
+        <v>28</v>
+      </c>
+      <c r="E23" s="3">
+        <v>1</v>
+      </c>
       <c r="F23" s="1">
-        <v>1985</v>
+        <v>2280</v>
       </c>
       <c r="G23" s="9"/>
       <c r="H23" s="6">
         <f t="shared" si="0"/>
-        <v>1384.6153846153848</v>
+        <v>2153.8461538461538</v>
       </c>
       <c r="I23" s="7">
         <f t="shared" si="1"/>
-        <v>0.43361111111111095</v>
+        <v>5.8571428571428587E-2</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1397,7 +1394,7 @@
         <v>35</v>
       </c>
       <c r="B24" s="1">
-        <v>1834</v>
+        <v>2113</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2">
@@ -1405,7 +1402,7 @@
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="1">
-        <v>1813</v>
+        <v>2092</v>
       </c>
       <c r="G24" s="10"/>
       <c r="H24" s="6">
@@ -1414,57 +1411,57 @@
       </c>
       <c r="I24" s="7">
         <f t="shared" si="1"/>
-        <v>0.2404736842105262</v>
+        <v>0.43136842105263146</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="5" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B25" s="1">
-        <v>1730</v>
+        <v>2012</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="1">
-        <v>1690</v>
-      </c>
-      <c r="G25" s="9"/>
+        <v>1964</v>
+      </c>
+      <c r="G25" s="10"/>
       <c r="H25" s="6">
         <f t="shared" si="0"/>
-        <v>2923.0769230769233</v>
+        <v>3538.4615384615386</v>
       </c>
       <c r="I25" s="7">
         <f t="shared" si="1"/>
-        <v>0.42184210526315796</v>
+        <v>0.44495652173913047</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="5" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B26" s="1">
-        <v>1706</v>
+        <v>1916</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="1">
-        <v>1663</v>
-      </c>
-      <c r="G26" s="10"/>
+        <v>1868</v>
+      </c>
+      <c r="G26" s="9"/>
       <c r="H26" s="6">
         <f t="shared" si="0"/>
-        <v>3153.8461538461538</v>
+        <v>3538.4615384615386</v>
       </c>
       <c r="I26" s="7">
         <f t="shared" si="1"/>
-        <v>0.47270731707317071</v>
+        <v>0.47208695652173915</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1472,24 +1469,24 @@
         <v>33</v>
       </c>
       <c r="B27" s="1">
-        <v>1598</v>
+        <v>1769</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="1">
-        <v>1563</v>
+        <v>1725</v>
       </c>
       <c r="G27" s="10"/>
       <c r="H27" s="6">
         <f t="shared" si="0"/>
-        <v>2461.5384615384614</v>
+        <v>3153.8461538461538</v>
       </c>
       <c r="I27" s="7">
         <f t="shared" si="1"/>
-        <v>0.36503124999999997</v>
+        <v>0.45304878048780489</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1497,32 +1494,32 @@
         <v>25</v>
       </c>
       <c r="B28" s="1">
-        <v>1554</v>
+        <v>1700</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="1">
-        <v>1523</v>
+        <v>1666</v>
       </c>
       <c r="G28" s="10"/>
       <c r="H28" s="6">
         <f t="shared" si="0"/>
-        <v>2384.6153846153848</v>
+        <v>2615.3846153846157</v>
       </c>
       <c r="I28" s="7">
         <f t="shared" si="1"/>
-        <v>0.36132258064516132</v>
+        <v>0.3630000000000001</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="5" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B29" s="1">
-        <v>1458</v>
+        <v>1515</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2">
@@ -1530,43 +1527,41 @@
       </c>
       <c r="E29" s="2"/>
       <c r="F29" s="1">
-        <v>1420</v>
-      </c>
-      <c r="G29" s="9"/>
+        <v>1477</v>
+      </c>
+      <c r="G29" s="10"/>
       <c r="H29" s="6">
         <f t="shared" si="0"/>
         <v>2923.0769230769233</v>
       </c>
       <c r="I29" s="7">
         <f t="shared" si="1"/>
-        <v>0.51421052631578956</v>
+        <v>0.49471052631578949</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B30" s="1">
-        <v>1270</v>
-      </c>
-      <c r="C30" s="4">
-        <v>9</v>
-      </c>
+        <v>1514</v>
+      </c>
+      <c r="C30" s="2"/>
       <c r="D30" s="2">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="1">
-        <v>1238</v>
-      </c>
-      <c r="G30" s="10"/>
+        <v>1442</v>
+      </c>
+      <c r="G30" s="9"/>
       <c r="H30" s="6">
         <f t="shared" si="0"/>
-        <v>2461.5384615384614</v>
+        <v>3307.6923076923076</v>
       </c>
       <c r="I30" s="7">
         <f t="shared" si="1"/>
-        <v>0.49706249999999996</v>
+        <v>0.56404651162790698</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1574,24 +1569,24 @@
         <v>30</v>
       </c>
       <c r="B31" s="1">
-        <v>1177</v>
+        <v>1358</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" s="1">
-        <v>1151</v>
+        <v>1329</v>
       </c>
       <c r="G31" s="10"/>
       <c r="H31" s="6">
         <f t="shared" si="0"/>
-        <v>2000</v>
+        <v>2230.7692307692309</v>
       </c>
       <c r="I31" s="7">
         <f t="shared" si="1"/>
-        <v>0.42449999999999999</v>
+        <v>0.40424137931034487</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1599,7 +1594,7 @@
         <v>28</v>
       </c>
       <c r="B32" s="1">
-        <v>1074</v>
+        <v>1246</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2">
@@ -1607,41 +1602,41 @@
       </c>
       <c r="E32" s="2"/>
       <c r="F32" s="1">
-        <v>1067</v>
-      </c>
-      <c r="G32" s="9"/>
+        <v>1239</v>
+      </c>
+      <c r="G32" s="10"/>
       <c r="H32" s="6">
         <f t="shared" si="0"/>
         <v>538.46153846153845</v>
       </c>
       <c r="I32" s="7">
         <f t="shared" si="1"/>
-        <v>0.98157142857142865</v>
+        <v>1.3009999999999999</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B33" s="2">
-        <v>891</v>
+      <c r="B33" s="1">
+        <v>1013</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E33" s="2"/>
-      <c r="F33" s="2">
-        <v>882</v>
+      <c r="F33" s="1">
+        <v>1003</v>
       </c>
       <c r="G33" s="9"/>
       <c r="H33" s="6">
         <f t="shared" si="0"/>
-        <v>692.30769230769238</v>
+        <v>769.23076923076928</v>
       </c>
       <c r="I33" s="7">
         <f t="shared" si="1"/>
-        <v>0.27399999999999985</v>
+        <v>0.30389999999999989</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1649,24 +1644,24 @@
         <v>46</v>
       </c>
       <c r="B34" s="2">
-        <v>879</v>
+        <v>988</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="2">
-        <v>844</v>
+        <v>949</v>
       </c>
       <c r="G34" s="10"/>
       <c r="H34" s="6">
         <f t="shared" si="0"/>
-        <v>2615.3846153846157</v>
+        <v>2923.0769230769233</v>
       </c>
       <c r="I34" s="7">
         <f t="shared" si="1"/>
-        <v>0.67729411764705882</v>
+        <v>0.67534210526315797</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1674,24 +1669,24 @@
         <v>37</v>
       </c>
       <c r="B35" s="2">
-        <v>826</v>
+        <v>899</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" s="2">
-        <v>805</v>
+        <v>877</v>
       </c>
       <c r="G35" s="9"/>
       <c r="H35" s="6">
         <f t="shared" si="0"/>
-        <v>1615.3846153846155</v>
+        <v>1692.3076923076924</v>
       </c>
       <c r="I35" s="7">
         <f t="shared" si="1"/>
-        <v>0.50166666666666671</v>
+        <v>0.4817727272727273</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1699,24 +1694,24 @@
         <v>38</v>
       </c>
       <c r="B36" s="2">
-        <v>770</v>
+        <v>831</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" s="2">
-        <v>675</v>
+        <v>730</v>
       </c>
       <c r="G36" s="9"/>
       <c r="H36" s="6">
         <f t="shared" si="0"/>
-        <v>2384.6153846153848</v>
+        <v>2846.1538461538462</v>
       </c>
       <c r="I36" s="7">
         <f t="shared" si="1"/>
-        <v>0.71693548387096773</v>
+        <v>0.74351351351351347</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1724,57 +1719,57 @@
         <v>32</v>
       </c>
       <c r="B37" s="2">
-        <v>742</v>
+        <v>789</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E37" s="2"/>
       <c r="F37" s="2">
-        <v>436</v>
+        <v>479</v>
       </c>
       <c r="G37" s="10"/>
       <c r="H37" s="6">
         <f t="shared" si="0"/>
-        <v>1384.6153846153848</v>
+        <v>1692.3076923076924</v>
       </c>
       <c r="I37" s="7">
         <f t="shared" si="1"/>
-        <v>0.68511111111111112</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>0.71695454545454551</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="5" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="B38" s="2">
-        <v>683</v>
+        <v>757</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" s="2">
-        <v>621</v>
-      </c>
-      <c r="G38" s="9"/>
+        <v>569</v>
+      </c>
+      <c r="G38" s="10"/>
       <c r="H38" s="6">
         <f t="shared" si="0"/>
-        <v>923.07692307692309</v>
+        <v>1153.8461538461538</v>
       </c>
       <c r="I38" s="7">
         <f t="shared" si="1"/>
-        <v>0.32724999999999999</v>
+        <v>0.50686666666666669</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="5" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B39" s="2">
-        <v>657</v>
+        <v>738</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2">
@@ -1782,7 +1777,7 @@
       </c>
       <c r="E39" s="2"/>
       <c r="F39" s="2">
-        <v>645</v>
+        <v>651</v>
       </c>
       <c r="G39" s="9"/>
       <c r="H39" s="6">
@@ -1791,32 +1786,32 @@
       </c>
       <c r="I39" s="7">
         <f t="shared" si="1"/>
-        <v>0.30125000000000002</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>0.29475000000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="5" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="B40" s="2">
-        <v>653</v>
+        <v>711</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" s="2">
-        <v>468</v>
-      </c>
-      <c r="G40" s="10"/>
+        <v>697</v>
+      </c>
+      <c r="G40" s="9"/>
       <c r="H40" s="6">
         <f t="shared" si="0"/>
-        <v>923.07692307692309</v>
+        <v>1076.9230769230769</v>
       </c>
       <c r="I40" s="7">
         <f t="shared" si="1"/>
-        <v>0.49299999999999999</v>
+        <v>0.35278571428571426</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1824,7 +1819,7 @@
         <v>41</v>
       </c>
       <c r="B41" s="2">
-        <v>614</v>
+        <v>699</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2">
@@ -1832,7 +1827,7 @@
       </c>
       <c r="E41" s="2"/>
       <c r="F41" s="2">
-        <v>585</v>
+        <v>670</v>
       </c>
       <c r="G41" s="9"/>
       <c r="H41" s="6">
@@ -1841,7 +1836,7 @@
       </c>
       <c r="I41" s="7">
         <f t="shared" si="1"/>
-        <v>0.30863636363636365</v>
+        <v>0.20818181818181822</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1849,24 +1844,24 @@
         <v>45</v>
       </c>
       <c r="B42" s="2">
-        <v>552</v>
+        <v>620</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E42" s="2"/>
       <c r="F42" s="2">
-        <v>539</v>
+        <v>603</v>
       </c>
       <c r="G42" s="9"/>
       <c r="H42" s="6">
         <f t="shared" si="0"/>
-        <v>1000</v>
+        <v>1307.6923076923078</v>
       </c>
       <c r="I42" s="7">
         <f t="shared" si="1"/>
-        <v>0.46100000000000002</v>
+        <v>0.53888235294117648</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1874,24 +1869,24 @@
         <v>42</v>
       </c>
       <c r="B43" s="2">
-        <v>479</v>
+        <v>540</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E43" s="2"/>
       <c r="F43" s="2">
-        <v>383</v>
+        <v>389</v>
       </c>
       <c r="G43" s="9"/>
       <c r="H43" s="6">
         <f t="shared" si="0"/>
-        <v>384.61538461538464</v>
+        <v>538.46153846153845</v>
       </c>
       <c r="I43" s="7">
         <f t="shared" si="1"/>
-        <v>4.2000000000000683E-3</v>
+        <v>0.27757142857142858</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1899,24 +1894,24 @@
         <v>44</v>
       </c>
       <c r="B44" s="2">
-        <v>403</v>
+        <v>495</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="2">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E44" s="2"/>
       <c r="F44" s="2">
-        <v>396</v>
+        <v>485</v>
       </c>
       <c r="G44" s="9"/>
       <c r="H44" s="6">
         <f t="shared" si="0"/>
-        <v>538.46153846153845</v>
+        <v>769.23076923076928</v>
       </c>
       <c r="I44" s="7">
         <f t="shared" si="1"/>
-        <v>0.26457142857142857</v>
+        <v>0.36950000000000005</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1924,24 +1919,24 @@
         <v>43</v>
       </c>
       <c r="B45" s="2">
-        <v>393</v>
+        <v>450</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E45" s="2"/>
       <c r="F45" s="2">
-        <v>332</v>
+        <v>365</v>
       </c>
       <c r="G45" s="9"/>
       <c r="H45" s="6">
         <f t="shared" si="0"/>
-        <v>923.07692307692309</v>
+        <v>1076.9230769230769</v>
       </c>
       <c r="I45" s="7">
         <f t="shared" si="1"/>
-        <v>0.64033333333333331</v>
+        <v>0.66107142857142853</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1949,24 +1944,24 @@
         <v>39</v>
       </c>
       <c r="B46" s="2">
-        <v>376</v>
+        <v>432</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E46" s="2"/>
       <c r="F46" s="2">
-        <v>275</v>
+        <v>310</v>
       </c>
       <c r="G46" s="9"/>
       <c r="H46" s="6">
         <f t="shared" si="0"/>
-        <v>538.46153846153845</v>
+        <v>692.30769230769238</v>
       </c>
       <c r="I46" s="7">
         <f t="shared" si="1"/>
-        <v>0.48928571428571427</v>
+        <v>0.55222222222222228</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1974,7 +1969,7 @@
         <v>48</v>
       </c>
       <c r="B47" s="2">
-        <v>338</v>
+        <v>389</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2">
@@ -1982,7 +1977,7 @@
       </c>
       <c r="E47" s="2"/>
       <c r="F47" s="2">
-        <v>321</v>
+        <v>372</v>
       </c>
       <c r="G47" s="10"/>
       <c r="H47" s="6">
@@ -1991,7 +1986,7 @@
       </c>
       <c r="I47" s="7">
         <f t="shared" si="1"/>
-        <v>0.75452941176470589</v>
+        <v>0.71552941176470597</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1999,24 +1994,24 @@
         <v>47</v>
       </c>
       <c r="B48" s="2">
-        <v>285</v>
+        <v>319</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E48" s="2"/>
       <c r="F48" s="2">
-        <v>226</v>
+        <v>258</v>
       </c>
       <c r="G48" s="10"/>
       <c r="H48" s="6">
         <f t="shared" si="0"/>
-        <v>76.92307692307692</v>
+        <v>230.76923076923077</v>
       </c>
       <c r="I48" s="7">
         <f t="shared" si="1"/>
-        <v>1.9380000000000004</v>
+        <v>0.11799999999999998</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2024,24 +2019,24 @@
         <v>50</v>
       </c>
       <c r="B49" s="2">
-        <v>246</v>
+        <v>279</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E49" s="2"/>
       <c r="F49" s="2">
-        <v>241</v>
+        <v>273</v>
       </c>
       <c r="G49" s="9"/>
       <c r="H49" s="6">
         <f t="shared" si="0"/>
-        <v>384.61538461538464</v>
+        <v>461.53846153846155</v>
       </c>
       <c r="I49" s="7">
         <f t="shared" si="1"/>
-        <v>0.37340000000000007</v>
+        <v>0.40850000000000003</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2049,17 +2044,15 @@
         <v>51</v>
       </c>
       <c r="B50" s="2">
-        <v>241</v>
-      </c>
-      <c r="C50" s="4">
-        <v>14</v>
-      </c>
+        <v>262</v>
+      </c>
+      <c r="C50" s="2"/>
       <c r="D50" s="2">
         <v>6</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" s="2">
-        <v>235</v>
+        <v>256</v>
       </c>
       <c r="G50" s="9"/>
       <c r="H50" s="6">
@@ -2068,7 +2061,7 @@
       </c>
       <c r="I50" s="7">
         <f t="shared" si="1"/>
-        <v>0.49083333333333334</v>
+        <v>0.44533333333333336</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2076,7 +2069,7 @@
         <v>56</v>
       </c>
       <c r="B51" s="2">
-        <v>217</v>
+        <v>237</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" s="2">
@@ -2084,7 +2077,7 @@
       </c>
       <c r="E51" s="2"/>
       <c r="F51" s="2">
-        <v>215</v>
+        <v>235</v>
       </c>
       <c r="G51" s="10"/>
       <c r="H51" s="6">
@@ -2093,7 +2086,7 @@
       </c>
       <c r="I51" s="7">
         <f t="shared" si="1"/>
-        <v>0.39750000000000008</v>
+        <v>0.52750000000000008</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2101,7 +2094,7 @@
         <v>54</v>
       </c>
       <c r="B52" s="2">
-        <v>165</v>
+        <v>187</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" s="2">
@@ -2109,7 +2102,7 @@
       </c>
       <c r="E52" s="2"/>
       <c r="F52" s="2">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="G52" s="10"/>
       <c r="H52" s="6">
@@ -2118,7 +2111,7 @@
       </c>
       <c r="I52" s="7">
         <f t="shared" si="1"/>
-        <v>0.31099999999999994</v>
+        <v>0.23949999999999996</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2126,7 +2119,7 @@
         <v>53</v>
       </c>
       <c r="B53" s="2">
-        <v>159</v>
+        <v>173</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2">
@@ -2134,7 +2127,7 @@
       </c>
       <c r="E53" s="2"/>
       <c r="F53" s="2">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="G53" s="10"/>
       <c r="H53" s="6">
@@ -2143,57 +2136,57 @@
       </c>
       <c r="I53" s="7">
         <f t="shared" si="1"/>
-        <v>0.51033333333333331</v>
+        <v>0.50166666666666671</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A54" s="5" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B54" s="2">
-        <v>151</v>
-      </c>
-      <c r="C54" s="4">
-        <v>8</v>
-      </c>
-      <c r="D54" s="2">
-        <v>3</v>
-      </c>
+        <v>166</v>
+      </c>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
       <c r="E54" s="2"/>
       <c r="F54" s="2">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="G54" s="9"/>
       <c r="H54" s="6">
         <f>D54/$I$1</f>
-        <v>230.76923076923077</v>
-      </c>
-      <c r="I54" s="7">
+        <v>0</v>
+      </c>
+      <c r="I54" s="7" t="e">
         <f>ABS(F54-H54)/H54</f>
-        <v>0.35866666666666669</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A55" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B55" s="2">
-        <v>150</v>
-      </c>
-      <c r="C55" s="2"/>
-      <c r="D55" s="2"/>
+        <v>157</v>
+      </c>
+      <c r="C55" s="4">
+        <v>6</v>
+      </c>
+      <c r="D55" s="2">
+        <v>3</v>
+      </c>
       <c r="E55" s="2"/>
       <c r="F55" s="2">
-        <v>124</v>
+        <v>154</v>
       </c>
       <c r="G55" s="9"/>
       <c r="H55" s="6">
         <f t="shared" ref="H55:H59" si="2">D55/$I$1</f>
-        <v>0</v>
-      </c>
-      <c r="I55" s="7" t="e">
+        <v>230.76923076923077</v>
+      </c>
+      <c r="I55" s="7">
         <f t="shared" ref="I55:I59" si="3">ABS(F55-H55)/H55</f>
-        <v>#DIV/0!</v>
+        <v>0.33266666666666667</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2205,20 +2198,20 @@
       </c>
       <c r="C56" s="2"/>
       <c r="D56" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E56" s="2"/>
       <c r="F56" s="2">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G56" s="9"/>
       <c r="H56" s="6">
         <f t="shared" si="2"/>
-        <v>230.76923076923077</v>
+        <v>307.69230769230768</v>
       </c>
       <c r="I56" s="7">
         <f t="shared" si="3"/>
-        <v>0.68800000000000006</v>
+        <v>0.76924999999999999</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -2251,24 +2244,24 @@
         <v>65</v>
       </c>
       <c r="B58" s="2">
-        <v>316</v>
+        <v>378</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" s="2">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E58" s="2"/>
       <c r="F58" s="2">
-        <v>300</v>
+        <v>359</v>
       </c>
       <c r="G58" s="9"/>
       <c r="H58" s="6">
         <f t="shared" si="2"/>
-        <v>923.07692307692309</v>
+        <v>1153.8461538461538</v>
       </c>
       <c r="I58" s="7">
         <f t="shared" si="3"/>
-        <v>0.67500000000000004</v>
+        <v>0.68886666666666663</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -2278,15 +2271,13 @@
       <c r="B59" s="18">
         <v>37</v>
       </c>
-      <c r="C59" s="22">
-        <v>7</v>
-      </c>
+      <c r="C59" s="18"/>
       <c r="D59" s="18"/>
       <c r="E59" s="18"/>
       <c r="F59" s="18">
         <v>8</v>
       </c>
-      <c r="G59" s="23"/>
+      <c r="G59" s="19"/>
       <c r="H59" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2316,7 +2307,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76AEA8A7-BC44-451F-9341-C0AE41AACCA3}">
   <dimension ref="A1:B56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>

</xml_diff>